<commit_message>
Pick last row number add row data
</commit_message>
<xml_diff>
--- a/dataset/Migrated Information/Migrated Samity.xlsx
+++ b/dataset/Migrated Information/Migrated Samity.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="26">
   <si>
     <t>Branch Code</t>
   </si>
@@ -78,6 +78,18 @@
   </si>
   <si>
     <t>001-009</t>
+  </si>
+  <si>
+    <t>222-011 - LAMP 1</t>
+  </si>
+  <si>
+    <t>222-012 - Dollan Chapa</t>
+  </si>
+  <si>
+    <t>222-013 - Golap</t>
+  </si>
+  <si>
+    <t>222-014 - Modhomoti</t>
   </si>
 </sst>
 </file>
@@ -122,7 +134,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -226,6 +238,90 @@
         <v>7</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>